<commit_message>
7º Commit: Adição de tratamento de dados no código com playwright.
</commit_message>
<xml_diff>
--- a/Web_Scraping_com_PlayWright/livros.xlsx
+++ b/Web_Scraping_com_PlayWright/livros.xlsx
@@ -134,6 +134,226 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Distribuição de Avaliações (Contagem)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sheet1'!B27</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet1'!$A$28:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$B$28:$B$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Avaliações (Estrelas)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Quantidade</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Percentual de Avaliações</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet1'!$A$28:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$C$28:$C$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="1"/>
+        </dLbls>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>42</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +669,11 @@
           <t>Quantidade</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Avaliação</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -462,6 +687,9 @@
       <c r="C2" t="n">
         <v>19</v>
       </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -475,6 +703,9 @@
       <c r="C3" t="n">
         <v>19</v>
       </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,6 +719,9 @@
       <c r="C4" t="n">
         <v>19</v>
       </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -501,6 +735,9 @@
       <c r="C5" t="n">
         <v>19</v>
       </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -514,6 +751,9 @@
       <c r="C6" t="n">
         <v>19</v>
       </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -527,6 +767,9 @@
       <c r="C7" t="n">
         <v>19</v>
       </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -540,6 +783,9 @@
       <c r="C8" t="n">
         <v>19</v>
       </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -553,6 +799,9 @@
       <c r="C9" t="n">
         <v>19</v>
       </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -566,6 +815,9 @@
       <c r="C10" t="n">
         <v>19</v>
       </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -579,6 +831,9 @@
       <c r="C11" t="n">
         <v>19</v>
       </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -592,6 +847,9 @@
       <c r="C12" t="n">
         <v>19</v>
       </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -605,6 +863,9 @@
       <c r="C13" t="n">
         <v>20</v>
       </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -618,6 +879,9 @@
       <c r="C14" t="n">
         <v>20</v>
       </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -631,6 +895,9 @@
       <c r="C15" t="n">
         <v>19</v>
       </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -644,6 +911,9 @@
       <c r="C16" t="n">
         <v>22</v>
       </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -657,6 +927,9 @@
       <c r="C17" t="n">
         <v>19</v>
       </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -670,6 +943,9 @@
       <c r="C18" t="n">
         <v>19</v>
       </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -683,6 +959,9 @@
       <c r="C19" t="n">
         <v>20</v>
       </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -696,6 +975,9 @@
       <c r="C20" t="n">
         <v>20</v>
       </c>
+      <c r="D20" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -709,8 +991,131 @@
       <c r="C21" t="n">
         <v>19</v>
       </c>
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Indicadores de Performance</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Percentual Bem Avaliados (%)</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Percentual Estoque Crítico (%)</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Preço Médio Bem Avaliados (£)</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>35.43</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Avaliação</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Contagem</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Percentual</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1 estrelas</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>6</v>
+      </c>
+      <c r="C28" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2 estrelas</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>3 estrelas</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>4 estrelas</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>5 estrelas</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" t="n">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>